<commit_message>
working - jusut need tto add appendix prompt
</commit_message>
<xml_diff>
--- a/data/OFFICIAL-TEST-SET-2.xlsx
+++ b/data/OFFICIAL-TEST-SET-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B71F5E1-BBA9-473B-88FE-4D728812B6F6}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C20339A-0444-468F-AC07-2E5E5E25C7C9}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="3015" windowWidth="23700" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8895" yWindow="600" windowWidth="14850" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
   <si>
     <t>Customer: 1038</t>
   </si>
@@ -408,25 +408,34 @@
     <t>Avg</t>
   </si>
   <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>2m</t>
+  </si>
+  <si>
+    <t>ld71r18u45aws</t>
+  </si>
+  <si>
+    <t>ld71r18u44lws</t>
+  </si>
+  <si>
+    <t>6m</t>
+  </si>
+  <si>
+    <t>8m</t>
+  </si>
+  <si>
+    <t>20m</t>
+  </si>
+  <si>
     <t>Analysis Window: Mon,Tue,Wed,Th,Fri, 20:00 to 08:00</t>
   </si>
   <si>
     <t>Data Pulled: Jun 09 2024 23:00:00 - Jun 21 2024 22:59:59</t>
   </si>
   <si>
-    <t>2m</t>
-  </si>
-  <si>
-    <t>10m</t>
-  </si>
-  <si>
-    <t>20m</t>
-  </si>
-  <si>
-    <t>6m</t>
-  </si>
-  <si>
-    <t>8m</t>
+    <t>ld71r18u44zws</t>
   </si>
 </sst>
 </file>
@@ -791,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -885,7 +894,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,6 +909,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1200,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN16"/>
+  <dimension ref="A1:BN19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:P4"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1225,7 @@
     <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="1" customWidth="1"/>
@@ -1270,7 +1282,7 @@
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1278,13 +1290,13 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2">
         <v>432000</v>
       </c>
     </row>
     <row r="3" spans="1:66" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -1594,7 +1606,7 @@
         <v>600</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J6" s="18">
         <v>1.3176204919673751E-2</v>
@@ -1612,7 +1624,7 @@
         <v>600</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P6" s="18"/>
       <c r="Q6" s="18">
@@ -1968,7 +1980,7 @@
         <v>360</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J8" s="18">
         <v>2.0376157407407001</v>
@@ -1986,7 +1998,7 @@
         <v>360</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="18">
@@ -2140,9 +2152,9 @@
         <v>1903922.5645696661</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="20">
@@ -2334,9 +2346,9 @@
         <v>874526.4324986093</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>80</v>
+    <row r="10" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="18">
@@ -2358,7 +2370,7 @@
         <v>480</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J10" s="18">
         <v>3.0224247685185301</v>
@@ -2530,9 +2542,9 @@
         <v>1922446.3413184991</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="20">
@@ -2554,7 +2566,7 @@
         <v>1200</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J11" s="20">
         <v>20.01953125</v>
@@ -2572,7 +2584,7 @@
         <v>1200</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P11" s="20"/>
       <c r="Q11" s="20">
@@ -2719,8 +2731,8 @@
       </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>82</v>
+      <c r="A12" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="18">
@@ -2742,7 +2754,7 @@
         <v>120</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J12" s="18">
         <v>6.6964285714306016E-2</v>
@@ -2760,7 +2772,7 @@
         <v>120</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="18">
@@ -2907,8 +2919,8 @@
       </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>83</v>
+      <c r="A13" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="20">
@@ -2934,10 +2946,10 @@
         <v>2.0978009259266631E-2</v>
       </c>
       <c r="K13" s="20">
-        <v>39.780673014322922</v>
+        <v>39.7806730143229</v>
       </c>
       <c r="L13" s="20">
-        <v>0.82103511441424359</v>
+        <v>4.82103511441424</v>
       </c>
       <c r="M13" s="20">
         <v>0</v>
@@ -3101,42 +3113,624 @@
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AA14" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB14">
-        <f>SUM(AB6:AB13)</f>
-        <v>10072.460556591883</v>
-      </c>
-      <c r="AC14">
-        <f>SUM(AC6:AC13)</f>
-        <v>31608.695045284487</v>
+      <c r="A14" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20">
+        <v>24</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0.27777777777778567</v>
+      </c>
+      <c r="E14" s="20">
+        <v>50.656376302083302</v>
+      </c>
+      <c r="F14" s="20">
+        <v>2.3885873544324698</v>
+      </c>
+      <c r="G14" s="20">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20">
+        <v>0</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20">
+        <v>2.0978009259266631E-2</v>
+      </c>
+      <c r="K14" s="20">
+        <v>59.7806730143229</v>
+      </c>
+      <c r="L14" s="20">
+        <v>3.82103511441424</v>
+      </c>
+      <c r="M14" s="20">
+        <v>0</v>
+      </c>
+      <c r="N14" s="20">
+        <v>0</v>
+      </c>
+      <c r="O14" s="20">
+        <v>0</v>
+      </c>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20">
+        <v>0</v>
+      </c>
+      <c r="R14" s="20">
+        <v>7.8579474317075722</v>
+      </c>
+      <c r="S14" s="20">
+        <v>10.41146600995569</v>
+      </c>
+      <c r="T14" s="20">
+        <v>7.9353826852469069</v>
+      </c>
+      <c r="U14" s="20">
+        <v>0</v>
+      </c>
+      <c r="V14" s="20">
+        <v>7.0431111111111098E-4</v>
+      </c>
+      <c r="W14" s="20">
+        <v>1.4554477777777779E-2</v>
+      </c>
+      <c r="X14" s="20">
+        <v>1.011656942132642E-3</v>
+      </c>
+      <c r="Y14" s="20">
+        <v>5.0999999999999993E-5</v>
+      </c>
+      <c r="Z14" s="20">
+        <v>6.150159999999999E-2</v>
+      </c>
+      <c r="AA14" s="20">
+        <v>1.285768816759496E-3</v>
+      </c>
+      <c r="AB14" s="20">
+        <v>216.13343850429229</v>
+      </c>
+      <c r="AC14" s="20">
+        <v>360.31434559116741</v>
+      </c>
+      <c r="AD14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="20">
+        <v>3.753968131666667E-3</v>
+      </c>
+      <c r="AF14" s="20">
+        <v>7.026705682098765E-5</v>
+      </c>
+      <c r="AG14" s="20">
+        <v>132.64664250167331</v>
+      </c>
+      <c r="AH14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="20">
+        <v>5.6379243499999991E-4</v>
+      </c>
+      <c r="AJ14" s="20">
+        <v>1.1130156265432099E-5</v>
+      </c>
+      <c r="AK14" s="20">
+        <v>16.06305184547217</v>
+      </c>
+      <c r="AL14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="20">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="AS14" s="20">
+        <v>44.173000000000002</v>
+      </c>
+      <c r="AT14" s="20">
+        <v>19.928370000000001</v>
+      </c>
+      <c r="AU14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="20">
+        <v>9</v>
+      </c>
+      <c r="AW14" s="20">
+        <v>45</v>
+      </c>
+      <c r="AX14" s="20">
+        <v>29.283018867924529</v>
+      </c>
+      <c r="AY14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ14" s="20">
+        <v>0</v>
+      </c>
+      <c r="BA14" s="20">
+        <v>2.413556622222222</v>
+      </c>
+      <c r="BB14" s="20">
+        <v>4.8563482469135791E-2</v>
+      </c>
+      <c r="BC14" s="20">
+        <v>5.5637333333333327E-3</v>
+      </c>
+      <c r="BD14" s="20">
+        <v>1.2283733333333331</v>
+      </c>
+      <c r="BE14" s="20">
+        <v>4.7060565205285308E-2</v>
+      </c>
+      <c r="BF14" s="20">
+        <v>0</v>
+      </c>
+      <c r="BG14" s="20">
+        <v>96.299999999999983</v>
+      </c>
+      <c r="BH14" s="20">
+        <v>1.939006512345679</v>
+      </c>
+      <c r="BI14" s="20">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="BJ14" s="20">
+        <v>74.35555555555554</v>
+      </c>
+      <c r="BK14" s="20">
+        <v>3.395697648219568</v>
+      </c>
+      <c r="BL14" s="20">
+        <v>1886902.02624</v>
+      </c>
+      <c r="BM14" s="20">
+        <v>1886946.0664319999</v>
+      </c>
+      <c r="BN14" s="20">
+        <v>1886943.3333380739</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AA15" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB15">
-        <f>AB14/F2</f>
-        <v>2.3315880918036765E-2</v>
-      </c>
-      <c r="AC15">
-        <f>AC14/F2</f>
-        <v>7.3168275567788169E-2</v>
+      <c r="A15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="20">
+        <v>24</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0.27777777777778567</v>
+      </c>
+      <c r="E15" s="20">
+        <v>30.656376302083299</v>
+      </c>
+      <c r="F15" s="20">
+        <v>3.3885873544324698</v>
+      </c>
+      <c r="G15" s="20">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
+        <v>0</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20">
+        <v>2.0978009259266631E-2</v>
+      </c>
+      <c r="K15" s="20">
+        <v>29.7806730143229</v>
+      </c>
+      <c r="L15" s="20">
+        <v>1.82103511441424</v>
+      </c>
+      <c r="M15" s="20">
+        <v>0</v>
+      </c>
+      <c r="N15" s="20">
+        <v>0</v>
+      </c>
+      <c r="O15" s="20">
+        <v>0</v>
+      </c>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20">
+        <v>0</v>
+      </c>
+      <c r="R15" s="20">
+        <v>7.8579474317075722</v>
+      </c>
+      <c r="S15" s="20">
+        <v>10.41146600995569</v>
+      </c>
+      <c r="T15" s="20">
+        <v>7.9353826852469069</v>
+      </c>
+      <c r="U15" s="20">
+        <v>0</v>
+      </c>
+      <c r="V15" s="20">
+        <v>7.0431111111111098E-4</v>
+      </c>
+      <c r="W15" s="20">
+        <v>1.4554477777777779E-2</v>
+      </c>
+      <c r="X15" s="20">
+        <v>1.011656942132642E-3</v>
+      </c>
+      <c r="Y15" s="20">
+        <v>5.0999999999999993E-5</v>
+      </c>
+      <c r="Z15" s="20">
+        <v>6.150159999999999E-2</v>
+      </c>
+      <c r="AA15" s="20">
+        <v>1.285768816759496E-3</v>
+      </c>
+      <c r="AB15" s="20">
+        <v>216.13343850429229</v>
+      </c>
+      <c r="AC15" s="20">
+        <v>360.31434559116741</v>
+      </c>
+      <c r="AD15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="20">
+        <v>3.753968131666667E-3</v>
+      </c>
+      <c r="AF15" s="20">
+        <v>7.026705682098765E-5</v>
+      </c>
+      <c r="AG15" s="20">
+        <v>132.64664250167331</v>
+      </c>
+      <c r="AH15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="20">
+        <v>5.6379243499999991E-4</v>
+      </c>
+      <c r="AJ15" s="20">
+        <v>1.1130156265432099E-5</v>
+      </c>
+      <c r="AK15" s="20">
+        <v>16.06305184547217</v>
+      </c>
+      <c r="AL15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="20">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="AS15" s="20">
+        <v>24.172999999999998</v>
+      </c>
+      <c r="AT15" s="20">
+        <v>5.9283700000000001</v>
+      </c>
+      <c r="AU15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="20">
+        <v>9</v>
+      </c>
+      <c r="AW15" s="20">
+        <v>45</v>
+      </c>
+      <c r="AX15" s="20">
+        <v>29.283018867924529</v>
+      </c>
+      <c r="AY15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="20">
+        <v>0</v>
+      </c>
+      <c r="BA15" s="20">
+        <v>2.413556622222222</v>
+      </c>
+      <c r="BB15" s="20">
+        <v>4.8563482469135791E-2</v>
+      </c>
+      <c r="BC15" s="20">
+        <v>5.5637333333333327E-3</v>
+      </c>
+      <c r="BD15" s="20">
+        <v>1.2283733333333331</v>
+      </c>
+      <c r="BE15" s="20">
+        <v>4.7060565205285308E-2</v>
+      </c>
+      <c r="BF15" s="20">
+        <v>0</v>
+      </c>
+      <c r="BG15" s="20">
+        <v>96.299999999999983</v>
+      </c>
+      <c r="BH15" s="20">
+        <v>1.939006512345679</v>
+      </c>
+      <c r="BI15" s="20">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="BJ15" s="20">
+        <v>74.35555555555554</v>
+      </c>
+      <c r="BK15" s="20">
+        <v>3.395697648219568</v>
+      </c>
+      <c r="BL15" s="20">
+        <v>1886902.02624</v>
+      </c>
+      <c r="BM15" s="20">
+        <v>1886946.0664319999</v>
+      </c>
+      <c r="BN15" s="20">
+        <v>1886943.3333380739</v>
       </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AA16" t="s">
+      <c r="A16" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="20">
+        <v>24</v>
+      </c>
+      <c r="D16" s="20">
+        <v>2.8193000000000001</v>
+      </c>
+      <c r="E16" s="20">
+        <v>75.656376302083302</v>
+      </c>
+      <c r="F16" s="20">
+        <v>61.388587354432403</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20">
+        <v>8.0209780092592595</v>
+      </c>
+      <c r="K16" s="20">
+        <v>79.7806730143229</v>
+      </c>
+      <c r="L16" s="20">
+        <v>69.821035114414201</v>
+      </c>
+      <c r="M16" s="20">
+        <v>0</v>
+      </c>
+      <c r="N16" s="20">
+        <v>0</v>
+      </c>
+      <c r="O16" s="20">
+        <v>0</v>
+      </c>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20">
+        <v>0</v>
+      </c>
+      <c r="R16" s="20">
+        <v>7.8579474317075722</v>
+      </c>
+      <c r="S16" s="20">
+        <v>10.41146600995569</v>
+      </c>
+      <c r="T16" s="20">
+        <v>7.9353826852469069</v>
+      </c>
+      <c r="U16" s="20">
+        <v>0</v>
+      </c>
+      <c r="V16" s="20">
+        <v>7.0431111111111098E-4</v>
+      </c>
+      <c r="W16" s="20">
+        <v>1.4554477777777779E-2</v>
+      </c>
+      <c r="X16" s="20">
+        <v>1.011656942132642E-3</v>
+      </c>
+      <c r="Y16" s="20">
+        <v>5.0999999999999993E-5</v>
+      </c>
+      <c r="Z16" s="20">
+        <v>6.150159999999999E-2</v>
+      </c>
+      <c r="AA16" s="20">
+        <v>1.285768816759496E-3</v>
+      </c>
+      <c r="AB16" s="20">
+        <v>216.13343850429229</v>
+      </c>
+      <c r="AC16" s="20">
+        <v>360.31434559116741</v>
+      </c>
+      <c r="AD16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="20">
+        <v>3.753968131666667E-3</v>
+      </c>
+      <c r="AF16" s="20">
+        <v>7.026705682098765E-5</v>
+      </c>
+      <c r="AG16" s="20">
+        <v>132.64664250167331</v>
+      </c>
+      <c r="AH16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="20">
+        <v>5.6379243499999991E-4</v>
+      </c>
+      <c r="AJ16" s="20">
+        <v>1.1130156265432099E-5</v>
+      </c>
+      <c r="AK16" s="20">
+        <v>16.06305184547217</v>
+      </c>
+      <c r="AL16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="20">
+        <v>20.137799999999999</v>
+      </c>
+      <c r="AS16" s="20">
+        <v>75.764300000000006</v>
+      </c>
+      <c r="AT16" s="20">
+        <v>59.987653999999999</v>
+      </c>
+      <c r="AU16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="20">
+        <v>9</v>
+      </c>
+      <c r="AW16" s="20">
+        <v>45</v>
+      </c>
+      <c r="AX16" s="20">
+        <v>29.283018867924529</v>
+      </c>
+      <c r="AY16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="20">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="20">
+        <v>2.413556622222222</v>
+      </c>
+      <c r="BB16" s="20">
+        <v>4.8563482469135791E-2</v>
+      </c>
+      <c r="BC16" s="20">
+        <v>5.5637333333333327E-3</v>
+      </c>
+      <c r="BD16" s="20">
+        <v>1.2283733333333331</v>
+      </c>
+      <c r="BE16" s="20">
+        <v>4.7060565205285308E-2</v>
+      </c>
+      <c r="BF16" s="20">
+        <v>0</v>
+      </c>
+      <c r="BG16" s="20">
+        <v>96.299999999999983</v>
+      </c>
+      <c r="BH16" s="20">
+        <v>1.939006512345679</v>
+      </c>
+      <c r="BI16" s="20">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="BJ16" s="20">
+        <v>74.35555555555554</v>
+      </c>
+      <c r="BK16" s="20">
+        <v>3.395697648219568</v>
+      </c>
+      <c r="BL16" s="20">
+        <v>1886902.02624</v>
+      </c>
+      <c r="BM16" s="20">
+        <v>1886946.0664319999</v>
+      </c>
+      <c r="BN16" s="20">
+        <v>1886943.3333380739</v>
+      </c>
+    </row>
+    <row r="17" spans="27:29" x14ac:dyDescent="0.25">
+      <c r="AA17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB17">
+        <f>SUM(AB6:AB16)</f>
+        <v>10720.860872104759</v>
+      </c>
+      <c r="AC17">
+        <f>SUM(AC6:AC16)</f>
+        <v>32689.638082057987</v>
+      </c>
+    </row>
+    <row r="18" spans="27:29" x14ac:dyDescent="0.25">
+      <c r="AA18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB18">
+        <f>AB17/F2</f>
+        <v>2.481680757431657E-2</v>
+      </c>
+      <c r="AC18">
+        <f>AC17/F2</f>
+        <v>7.5670458523282372E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="27:29" x14ac:dyDescent="0.25">
+      <c r="AA19" t="s">
         <v>86</v>
       </c>
-      <c r="AB16">
-        <f>AB14/8/F2</f>
-        <v>2.9144851147545957E-3</v>
-      </c>
-      <c r="AC16">
-        <f>AC14/8/F2</f>
-        <v>9.1460344459735211E-3</v>
+      <c r="AB19">
+        <f>AB17/8/F2</f>
+        <v>3.1021009467895712E-3</v>
+      </c>
+      <c r="AC19">
+        <f>AC17/8/F2</f>
+        <v>9.4588073154102965E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Self contained and read me done!
</commit_message>
<xml_diff>
--- a/data/OFFICIAL-TEST-SET-2.xlsx
+++ b/data/OFFICIAL-TEST-SET-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C20339A-0444-468F-AC07-2E5E5E25C7C9}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C13C4BA8-C246-483A-81AB-CC327F6FEE0F}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="600" windowWidth="14850" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -796,11 +796,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -870,9 +894,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -892,6 +913,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,8 +1278,8 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="1" customWidth="1"/>
@@ -1303,61 +1357,61 @@
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="39" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="27" t="s">
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="31" t="s">
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="53"/>
+      <c r="Z4" s="53"/>
+      <c r="AA4" s="53"/>
+      <c r="AB4" s="53"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="23"/>
-      <c r="AL4" s="23"/>
-      <c r="AM4" s="23"/>
-      <c r="AN4" s="23"/>
-      <c r="AO4" s="23"/>
-      <c r="AP4" s="23"/>
-      <c r="AQ4" s="24"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="50"/>
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="50"/>
+      <c r="AJ4" s="50"/>
+      <c r="AK4" s="50"/>
+      <c r="AL4" s="50"/>
+      <c r="AM4" s="50"/>
+      <c r="AN4" s="50"/>
+      <c r="AO4" s="50"/>
+      <c r="AP4" s="50"/>
+      <c r="AQ4" s="51"/>
       <c r="AR4" s="29" t="s">
         <v>10</v>
       </c>
@@ -1387,8 +1441,8 @@
       <c r="BN4" s="26"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -3820,29 +3874,29 @@
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="39" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="38" t="s">
         <v>7</v>
       </c>
       <c r="R4" s="26"/>
@@ -3861,8 +3915,8 @@
       <c r="AC4" s="28"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -4311,26 +4365,26 @@
       <c r="BN3" s="1"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="44" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="43" t="s">
         <v>92</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="14" t="s">
         <v>93</v>
       </c>

</xml_diff>